<commit_message>
feat: load images in xlsx
</commit_message>
<xml_diff>
--- a/server/data_parser/tests/assets/test.xlsx
+++ b/server/data_parser/tests/assets/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\develop\Excel-Compare-and-Import\server\data_parser\tests\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8D94B6-E513-4174-AFA1-1740D49D4305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E09F8E3-5F05-4DF8-AFFF-61665A1F3B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,48 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="3">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="3">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+  </valueMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -109,59 +151,78 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>34516</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>623162</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>847726</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DDB73FB-9D28-9974-F343-694F657B06AD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2839629" y="438150"/>
-          <a:ext cx="588646" cy="762001"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -427,18 +488,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="12.06640625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="99.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,6 +510,9 @@
       <c r="C1" s="1"/>
       <c r="D1" t="s">
         <v>2</v>
+      </c>
+      <c r="E1" t="e" vm="1">
+        <v>#VALUE!</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -468,6 +533,9 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="E3" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="F3">
         <v>19</v>
       </c>
@@ -478,6 +546,11 @@
       </c>
       <c r="F4">
         <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E8" t="e" vm="3">
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -486,6 +559,5 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>